<commit_message>
Renamed Recall->Retrieval, changed number blocks and corrected condition files
</commit_message>
<xml_diff>
--- a/Recall/Retrieval_names.xlsx
+++ b/Recall/Retrieval_names.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lunduniversityo365-my.sharepoint.com/personal/pi6342kl_lu_se/Documents/Biofinder/fMRI-tasks/FacesNamesProfessions_fMRI/Recall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="11_F25DC773A252ABDACC1048BC415F7C7A5ADE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7DD9E52-AB27-4C80-A020-5EC9507A2132}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="11_F25DC773A252ABDACC1048BC415F7C7A5ADE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD0702C5-2918-48F4-8B9D-8E95D37C77A4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="76">
   <si>
     <t>StimFile</t>
   </si>
@@ -230,67 +230,40 @@
     <t>Images_Faces/O51.jpg</t>
   </si>
   <si>
-    <t>Simon</t>
-  </si>
-  <si>
     <t>Images_Faces/O52.jpg</t>
   </si>
   <si>
-    <t>Håkan</t>
-  </si>
-  <si>
     <t>Images_Faces/O53.jpg</t>
   </si>
   <si>
-    <t>Christoffer</t>
-  </si>
-  <si>
     <t>Images_Faces/O54.jpg</t>
   </si>
   <si>
-    <t>Rickard</t>
-  </si>
-  <si>
     <t>Images_Faces/O55.jpg</t>
   </si>
   <si>
-    <t>Kjell</t>
-  </si>
-  <si>
     <t>Images_Faces/O56.jpg</t>
   </si>
   <si>
-    <t>William</t>
-  </si>
-  <si>
     <t>Images_Faces/O57.jpg</t>
   </si>
   <si>
-    <t>Joakim</t>
-  </si>
-  <si>
     <t>Images_Faces/O58.jpg</t>
   </si>
   <si>
-    <t>Stig</t>
-  </si>
-  <si>
     <t>Images_Faces/O59.jpg</t>
   </si>
   <si>
-    <t>Anton</t>
-  </si>
-  <si>
     <t>Images_Faces/O60.jpg</t>
   </si>
   <si>
-    <t>Wilhelm</t>
-  </si>
-  <si>
     <t>task</t>
   </si>
   <si>
     <t>Profession</t>
+  </si>
+  <si>
+    <t>NY</t>
   </si>
 </sst>
 </file>
@@ -354,10 +327,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -625,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32:C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,7 +606,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -646,7 +615,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1077,7 +1046,7 @@
         <v>63</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -1088,10 +1057,10 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1102,10 +1071,10 @@
         <v>2</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -1116,10 +1085,10 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C35" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -1130,10 +1099,10 @@
         <v>2</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -1144,10 +1113,10 @@
         <v>2</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -1158,10 +1127,10 @@
         <v>2</v>
       </c>
       <c r="B38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" t="s">
         <v>75</v>
-      </c>
-      <c r="C38" t="s">
-        <v>76</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -1172,10 +1141,10 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C39" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -1186,10 +1155,10 @@
         <v>2</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -1200,10 +1169,10 @@
         <v>2</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D41">
         <v>0</v>

</xml_diff>